<commit_message>
local vol calibration main
</commit_message>
<xml_diff>
--- a/source/LocVol Parameters.xlsx
+++ b/source/LocVol Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\van92\OneDrive\Desktop\Local-Vol-Calibration\source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mymurex-my.sharepoint.com/personal/ycui_murex_com/Documents/Desktop/Local Vol Calibration/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747663E7-DE4B-494D-AE00-F3244F1EDAD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1455" windowWidth="14250" windowHeight="12930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-990" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IRSMFORM" sheetId="1" r:id="rId1"/>
@@ -330,7 +330,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
-    <numFmt numFmtId="173" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -703,13 +703,13 @@
     <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -24629,7 +24629,7 @@
   <dimension ref="B1:X79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="V35" sqref="V35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24640,7 +24640,7 @@
       </c>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="43">
+      <c r="B2" s="41">
         <v>1.0822999976901</v>
       </c>
     </row>
@@ -24721,815 +24721,815 @@
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="43">
+      <c r="B6" s="41">
         <v>2.7397260273999999E-3</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C6" s="41">
         <v>4.1155828699999996E-3</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="41">
         <v>2.7397260273999999E-3</v>
       </c>
-      <c r="F6" s="43">
+      <c r="F6" s="41">
         <v>-4.5584587960999998E-3</v>
       </c>
-      <c r="H6" s="43">
+      <c r="H6" s="41">
         <v>2.7397260273999999E-3</v>
       </c>
-      <c r="I6" s="43">
+      <c r="I6" s="41">
         <v>-3.4420062715500001E-2</v>
       </c>
-      <c r="K6" s="43">
+      <c r="K6" s="41">
         <v>2.7397260273999999E-3</v>
       </c>
-      <c r="L6" s="43">
+      <c r="L6" s="41">
         <v>0.13500000000000001</v>
       </c>
-      <c r="N6" s="43">
+      <c r="N6" s="41">
         <v>1.0928611436024001</v>
       </c>
-      <c r="O6" s="43">
+      <c r="O6" s="41">
         <v>1.0877712353913001</v>
       </c>
-      <c r="P6" s="43">
+      <c r="P6" s="41">
         <v>1.0824548120705999</v>
       </c>
-      <c r="Q6" s="43">
+      <c r="Q6" s="41">
         <v>1.0773555473554</v>
       </c>
-      <c r="R6" s="43">
+      <c r="R6" s="41">
         <v>1.0727260244829</v>
       </c>
-      <c r="T6" s="43">
+      <c r="T6" s="41">
         <v>0.1425855308592</v>
       </c>
-      <c r="U6" s="43">
+      <c r="U6" s="41">
         <v>0.1387265831765</v>
       </c>
-      <c r="V6" s="43">
+      <c r="V6" s="41">
         <v>0.13500000000000001</v>
       </c>
-      <c r="W6" s="43">
+      <c r="W6" s="41">
         <v>0.13372658317649999</v>
       </c>
-      <c r="X6" s="43">
+      <c r="X6" s="41">
         <v>0.1345855308592</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="43">
+      <c r="B7" s="41">
         <v>5.4794520547999997E-3</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="41">
         <v>5.2824232969999997E-3</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="41">
         <v>5.4794520547999997E-3</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="41">
         <v>-9.7565457365999999E-3</v>
       </c>
-      <c r="H7" s="43">
+      <c r="H7" s="41">
         <v>5.4794520547999997E-3</v>
       </c>
-      <c r="I7" s="43">
+      <c r="I7" s="41">
         <v>-1.1036046175E-2</v>
       </c>
-      <c r="K7" s="43">
+      <c r="K7" s="41">
         <v>1.9178082191799999E-2</v>
       </c>
-      <c r="L7" s="43">
+      <c r="L7" s="41">
         <v>0.114</v>
       </c>
-      <c r="N7" s="43">
+      <c r="N7" s="41">
         <v>1.1060402313711</v>
       </c>
-      <c r="O7" s="43">
+      <c r="O7" s="41">
         <v>1.0945434918243999</v>
       </c>
-      <c r="P7" s="43">
+      <c r="P7" s="41">
         <v>1.0826422175114001</v>
       </c>
-      <c r="Q7" s="43">
+      <c r="Q7" s="41">
         <v>1.0712263148159</v>
       </c>
-      <c r="R7" s="43">
+      <c r="R7" s="41">
         <v>1.0608100596131</v>
       </c>
-      <c r="T7" s="43">
+      <c r="T7" s="41">
         <v>0.1203924027461</v>
       </c>
-      <c r="U7" s="43">
+      <c r="U7" s="41">
         <v>0.1169658277874</v>
       </c>
-      <c r="V7" s="43">
+      <c r="V7" s="41">
         <v>0.114</v>
       </c>
-      <c r="W7" s="43">
+      <c r="W7" s="41">
         <v>0.1134658277874</v>
       </c>
-      <c r="X7" s="43">
+      <c r="X7" s="41">
         <v>0.1147924027461</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="43">
+      <c r="B8" s="41">
         <v>1.3698630137E-2</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="41">
         <v>5.9825275532000002E-3</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="41">
         <v>1.3698630137E-2</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="41">
         <v>-8.6518809365999996E-3</v>
       </c>
-      <c r="H8" s="43">
+      <c r="H8" s="41">
         <v>1.3698630137E-2</v>
       </c>
-      <c r="I8" s="43">
+      <c r="I8" s="41">
         <v>2.8758179006000001E-3</v>
       </c>
-      <c r="K8" s="43">
+      <c r="K8" s="41">
         <v>3.8356164383599997E-2</v>
       </c>
-      <c r="L8" s="43">
+      <c r="L8" s="41">
         <v>0.1055</v>
       </c>
-      <c r="N8" s="43">
+      <c r="N8" s="41">
         <v>1.1138330420706</v>
       </c>
-      <c r="O8" s="43">
+      <c r="O8" s="41">
         <v>1.0985408873741001</v>
       </c>
-      <c r="P8" s="43">
+      <c r="P8" s="41">
         <v>1.0829283667131999</v>
       </c>
-      <c r="Q8" s="43">
+      <c r="Q8" s="41">
         <v>1.0679035858624</v>
       </c>
-      <c r="R8" s="43">
+      <c r="R8" s="41">
         <v>1.0539781449123</v>
       </c>
-      <c r="T8" s="43">
+      <c r="T8" s="41">
         <v>0.1119965744464</v>
       </c>
-      <c r="U8" s="43">
+      <c r="U8" s="41">
         <v>0.1082591241115</v>
       </c>
-      <c r="V8" s="43">
+      <c r="V8" s="41">
         <v>0.1055</v>
       </c>
-      <c r="W8" s="43">
+      <c r="W8" s="41">
         <v>0.1057591241115</v>
       </c>
-      <c r="X8" s="43">
+      <c r="X8" s="41">
         <v>0.1079965744464</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B9" s="43">
+      <c r="B9" s="41">
         <v>1.9178082191799999E-2</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="41">
         <v>6.1158807448000001E-3</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="41">
         <v>1.9178082191799999E-2</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="41">
         <v>-6.5799608283999998E-3</v>
       </c>
-      <c r="H9" s="43">
+      <c r="H9" s="41">
         <v>1.9178082191799999E-2</v>
       </c>
-      <c r="I9" s="43">
+      <c r="I9" s="41">
         <v>2.7090418631E-3</v>
       </c>
-      <c r="K9" s="43">
+      <c r="K9" s="41">
         <v>7.9452054794500002E-2</v>
       </c>
-      <c r="L9" s="43">
+      <c r="L9" s="41">
         <v>0.10349999999999999</v>
       </c>
-      <c r="N9" s="43">
+      <c r="N9" s="41">
         <v>1.127924371722</v>
       </c>
-      <c r="O9" s="43">
+      <c r="O9" s="41">
         <v>1.1057243779239001</v>
       </c>
-      <c r="P9" s="43">
+      <c r="P9" s="41">
         <v>1.0836344624465</v>
       </c>
-      <c r="Q9" s="43">
+      <c r="Q9" s="41">
         <v>1.0622231744132999</v>
       </c>
-      <c r="R9" s="43">
+      <c r="R9" s="41">
         <v>1.0418062745665999</v>
       </c>
-      <c r="T9" s="43">
+      <c r="T9" s="41">
         <v>0.1107107890606</v>
       </c>
-      <c r="U9" s="43">
+      <c r="U9" s="41">
         <v>0.1060020825058</v>
       </c>
-      <c r="V9" s="43">
+      <c r="V9" s="41">
         <v>0.10349999999999999</v>
       </c>
-      <c r="W9" s="43">
+      <c r="W9" s="41">
         <v>0.1050020825058</v>
       </c>
-      <c r="X9" s="43">
+      <c r="X9" s="41">
         <v>0.1090907890606</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B10" s="43">
+      <c r="B10" s="41">
         <v>2.4657534246599999E-2</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="41">
         <v>6.1899658512999996E-3</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="41">
         <v>2.4657534246599999E-2</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="41">
         <v>-4.919538153E-3</v>
       </c>
-      <c r="H10" s="43">
+      <c r="H10" s="41">
         <v>2.4657534246599999E-2</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="41">
         <v>-3.6304132390000001E-4</v>
       </c>
-      <c r="K10" s="43">
+      <c r="K10" s="41">
         <v>0.158904109589</v>
       </c>
-      <c r="L10" s="43">
+      <c r="L10" s="41">
         <v>0.11250499999999999</v>
       </c>
-      <c r="N10" s="43">
+      <c r="N10" s="41">
         <v>1.1538059215845</v>
       </c>
-      <c r="O10" s="43">
+      <c r="O10" s="41">
         <v>1.1192192492705</v>
       </c>
-      <c r="P10" s="43">
+      <c r="P10" s="41">
         <v>1.0852981845758001</v>
       </c>
-      <c r="Q10" s="43">
+      <c r="Q10" s="41">
         <v>1.0520756891312</v>
       </c>
-      <c r="R10" s="43">
+      <c r="R10" s="41">
         <v>1.0198978458435</v>
       </c>
-      <c r="T10" s="43">
+      <c r="T10" s="41">
         <v>0.11952873647789999</v>
       </c>
-      <c r="U10" s="43">
+      <c r="U10" s="41">
         <v>0.114255558912</v>
       </c>
-      <c r="V10" s="43">
+      <c r="V10" s="41">
         <v>0.11250499999999999</v>
       </c>
-      <c r="W10" s="43">
+      <c r="W10" s="41">
         <v>0.115755558912</v>
       </c>
-      <c r="X10" s="43">
+      <c r="X10" s="41">
         <v>0.12196873647790001</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B11" s="43">
+      <c r="B11" s="41">
         <v>3.8356164383599997E-2</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="41">
         <v>6.2825722343999996E-3</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="41">
         <v>3.8356164383599997E-2</v>
       </c>
-      <c r="F11" s="43">
+      <c r="F11" s="41">
         <v>-3.9785812372000002E-3</v>
       </c>
-      <c r="H11" s="43">
+      <c r="H11" s="41">
         <v>3.8356164383599997E-2</v>
       </c>
-      <c r="I11" s="43">
+      <c r="I11" s="41">
         <v>6.9394524460000004E-4</v>
       </c>
-      <c r="K11" s="43">
+      <c r="K11" s="41">
         <v>0.24657534246580001</v>
       </c>
-      <c r="L11" s="43">
+      <c r="L11" s="41">
         <v>0.11125500000000001</v>
       </c>
-      <c r="N11" s="43">
+      <c r="N11" s="41">
         <v>1.1714163164200999</v>
       </c>
-      <c r="O11" s="43">
+      <c r="O11" s="41">
         <v>1.1286745281187001</v>
       </c>
-      <c r="P11" s="43">
+      <c r="P11" s="41">
         <v>1.0869020003701</v>
       </c>
-      <c r="Q11" s="43">
+      <c r="Q11" s="41">
         <v>1.0457747662464001</v>
       </c>
-      <c r="R11" s="43">
+      <c r="R11" s="41">
         <v>1.0058038539642</v>
       </c>
-      <c r="T11" s="43">
+      <c r="T11" s="41">
         <v>0.1173419741591</v>
       </c>
-      <c r="U11" s="43">
+      <c r="U11" s="41">
         <v>0.11236048733120001</v>
       </c>
-      <c r="V11" s="43">
+      <c r="V11" s="41">
         <v>0.11125500000000001</v>
       </c>
-      <c r="W11" s="43">
+      <c r="W11" s="41">
         <v>0.1153604873312</v>
       </c>
-      <c r="X11" s="43">
+      <c r="X11" s="41">
         <v>0.12229197415909999</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B12" s="43">
+      <c r="B12" s="41">
         <v>4.3835616438399998E-2</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="41">
         <v>6.3034086705999999E-3</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="41">
         <v>4.3835616438399998E-2</v>
       </c>
-      <c r="F12" s="43">
+      <c r="F12" s="41">
         <v>-3.9477696572000004E-3</v>
       </c>
-      <c r="H12" s="43">
+      <c r="H12" s="41">
         <v>4.3835616438399998E-2</v>
       </c>
-      <c r="I12" s="43">
+      <c r="I12" s="41">
         <v>-4.1125478679999999E-4</v>
       </c>
-      <c r="K12" s="43">
+      <c r="K12" s="41">
         <v>0.49863013698629999</v>
       </c>
-      <c r="L12" s="43">
+      <c r="L12" s="41">
         <v>0.108505</v>
       </c>
-      <c r="N12" s="43">
+      <c r="N12" s="41">
         <v>1.2097180230955</v>
       </c>
-      <c r="O12" s="43">
+      <c r="O12" s="41">
         <v>1.1500061624697999</v>
       </c>
-      <c r="P12" s="43">
+      <c r="P12" s="41">
         <v>1.0919900365121</v>
       </c>
-      <c r="Q12" s="43">
+      <c r="Q12" s="41">
         <v>1.0343691196021001</v>
       </c>
-      <c r="R12" s="43">
+      <c r="R12" s="41">
         <v>0.97804090244789998</v>
       </c>
-      <c r="T12" s="43">
+      <c r="T12" s="41">
         <v>0.11274331937199999</v>
       </c>
-      <c r="U12" s="43">
+      <c r="U12" s="41">
         <v>0.1083566959254</v>
       </c>
-      <c r="V12" s="43">
+      <c r="V12" s="41">
         <v>0.108505</v>
       </c>
-      <c r="W12" s="43">
+      <c r="W12" s="41">
         <v>0.1141066959254</v>
       </c>
-      <c r="X12" s="43">
+      <c r="X12" s="41">
         <v>0.12252331937200001</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B13" s="43">
+      <c r="B13" s="41">
         <v>6.3013698630100007E-2</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="41">
         <v>6.3477993390000003E-3</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="41">
         <v>6.3013698630100007E-2</v>
       </c>
-      <c r="F13" s="43">
+      <c r="F13" s="41">
         <v>-3.6443324806E-3</v>
       </c>
-      <c r="H13" s="43">
+      <c r="H13" s="41">
         <v>6.3013698630100007E-2</v>
       </c>
-      <c r="I13" s="43">
+      <c r="I13" s="41">
         <v>-7.661678842E-4</v>
       </c>
-      <c r="K13" s="43">
+      <c r="K13" s="41">
         <v>0.75068493150680005</v>
       </c>
-      <c r="L13" s="43">
+      <c r="L13" s="41">
         <v>0.10860499999999999</v>
       </c>
-      <c r="N13" s="43">
+      <c r="N13" s="41">
         <v>1.2441955366813</v>
       </c>
-      <c r="O13" s="43">
+      <c r="O13" s="41">
         <v>1.1694135421633001</v>
       </c>
-      <c r="P13" s="43">
+      <c r="P13" s="41">
         <v>1.0975273849255001</v>
       </c>
-      <c r="Q13" s="43">
+      <c r="Q13" s="41">
         <v>1.0264727609905</v>
       </c>
-      <c r="R13" s="43">
+      <c r="R13" s="41">
         <v>0.95744594483519996</v>
       </c>
-      <c r="T13" s="43">
+      <c r="T13" s="41">
         <v>0.112448036487</v>
       </c>
-      <c r="U13" s="43">
+      <c r="U13" s="41">
         <v>0.1080641976553</v>
       </c>
-      <c r="V13" s="43">
+      <c r="V13" s="41">
         <v>0.10860499999999999</v>
       </c>
-      <c r="W13" s="43">
+      <c r="W13" s="41">
         <v>0.1148141976553</v>
       </c>
-      <c r="X13" s="43">
+      <c r="X13" s="41">
         <v>0.123928036487</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="43">
+      <c r="B14" s="41">
         <v>7.9452054794500002E-2</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="41">
         <v>6.3687919704000003E-3</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="41">
         <v>7.9452054794500002E-2</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="41">
         <v>-3.9756211484000001E-3</v>
       </c>
-      <c r="H14" s="43">
+      <c r="H14" s="41">
         <v>7.9452054794500002E-2</v>
       </c>
-      <c r="I14" s="43">
+      <c r="I14" s="41">
         <v>1.9143389140000001E-4</v>
       </c>
-      <c r="K14" s="43">
+      <c r="K14" s="41">
         <v>1</v>
       </c>
-      <c r="L14" s="43">
+      <c r="L14" s="41">
         <v>0.1085</v>
       </c>
-      <c r="N14" s="43">
+      <c r="N14" s="41">
         <v>1.2755193361949999</v>
       </c>
-      <c r="O14" s="43">
+      <c r="O14" s="41">
         <v>1.1872917704288</v>
       </c>
-      <c r="P14" s="43">
+      <c r="P14" s="41">
         <v>1.1034778960942999</v>
       </c>
-      <c r="Q14" s="43">
+      <c r="Q14" s="41">
         <v>1.0212114692365999</v>
       </c>
-      <c r="R14" s="43">
+      <c r="R14" s="41">
         <v>0.94181387711169995</v>
       </c>
-      <c r="T14" s="43">
+      <c r="T14" s="41">
         <v>0.11238719204600001</v>
       </c>
-      <c r="U14" s="43">
+      <c r="U14" s="41">
         <v>0.10781054407689999</v>
       </c>
-      <c r="V14" s="43">
+      <c r="V14" s="41">
         <v>0.1085</v>
       </c>
-      <c r="W14" s="43">
+      <c r="W14" s="41">
         <v>0.1150605440769</v>
       </c>
-      <c r="X14" s="43">
+      <c r="X14" s="41">
         <v>0.124717192046</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="43">
+      <c r="B15" s="41">
         <v>9.0410958904100003E-2</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="41">
         <v>6.3785461222999997E-3</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="41">
         <v>9.0410958904100003E-2</v>
       </c>
-      <c r="F15" s="43">
+      <c r="F15" s="41">
         <v>-3.4552216250000002E-3</v>
       </c>
-      <c r="H15" s="43">
+      <c r="H15" s="41">
         <v>9.0410958904100003E-2</v>
       </c>
-      <c r="I15" s="43">
+      <c r="I15" s="41">
         <v>8.8081881799999999E-4</v>
       </c>
-      <c r="K15" s="43">
+      <c r="K15" s="41">
         <v>1.9972602739726</v>
       </c>
-      <c r="L15" s="43">
+      <c r="L15" s="41">
         <v>0.108</v>
       </c>
-      <c r="N15" s="43">
+      <c r="N15" s="41">
         <v>1.3753185664284</v>
       </c>
-      <c r="O15" s="43">
+      <c r="O15" s="41">
         <v>1.2424486597266999</v>
       </c>
-      <c r="P15" s="43">
+      <c r="P15" s="41">
         <v>1.1215384780538999</v>
       </c>
-      <c r="Q15" s="43">
+      <c r="Q15" s="41">
         <v>1.0073796800739001</v>
       </c>
-      <c r="R15" s="43">
+      <c r="R15" s="41">
         <v>0.90042792496390001</v>
       </c>
-      <c r="T15" s="43">
+      <c r="T15" s="41">
         <v>0.1121262326205</v>
       </c>
-      <c r="U15" s="43">
+      <c r="U15" s="41">
         <v>0.1075165547746</v>
       </c>
-      <c r="V15" s="43">
+      <c r="V15" s="41">
         <v>0.108</v>
       </c>
-      <c r="W15" s="43">
+      <c r="W15" s="41">
         <v>0.1140165547746</v>
       </c>
-      <c r="X15" s="43">
+      <c r="X15" s="41">
         <v>0.1231762326205</v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="43">
+      <c r="B16" s="41">
         <v>9.5890410958899996E-2</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="41">
         <v>6.3825871280999997E-3</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="41">
         <v>9.5890410958899996E-2</v>
       </c>
-      <c r="F16" s="43">
+      <c r="F16" s="41">
         <v>-2.9181343786000001E-3</v>
       </c>
-      <c r="H16" s="43">
+      <c r="H16" s="41">
         <v>9.5890410958899996E-2</v>
       </c>
-      <c r="I16" s="43">
+      <c r="I16" s="41">
         <v>5.2882358600000003E-4</v>
       </c>
-      <c r="K16" s="43">
+      <c r="K16" s="41">
         <v>2.9972602739726</v>
       </c>
-      <c r="L16" s="43">
+      <c r="L16" s="41">
         <v>0.11</v>
       </c>
-      <c r="N16" s="43">
+      <c r="N16" s="41">
         <v>1.4851170685057</v>
       </c>
-      <c r="O16" s="43">
+      <c r="O16" s="41">
         <v>1.3033626022547999</v>
       </c>
-      <c r="P16" s="43">
+      <c r="P16" s="41">
         <v>1.1450649183521</v>
       </c>
-      <c r="Q16" s="43">
+      <c r="Q16" s="41">
         <v>1.0031181012804999</v>
       </c>
-      <c r="R16" s="43">
+      <c r="R16" s="41">
         <v>0.87547900670870005</v>
       </c>
-      <c r="T16" s="43">
+      <c r="T16" s="41">
         <v>0.1162458703394</v>
       </c>
-      <c r="U16" s="43">
+      <c r="U16" s="41">
         <v>0.1106922774384</v>
       </c>
-      <c r="V16" s="43">
+      <c r="V16" s="41">
         <v>0.11</v>
       </c>
-      <c r="W16" s="43">
+      <c r="W16" s="41">
         <v>0.11469227743840001</v>
       </c>
-      <c r="X16" s="43">
+      <c r="X16" s="41">
         <v>0.1230458703394</v>
       </c>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B17" s="43">
+      <c r="B17" s="41">
         <v>0.1369863013699</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="41">
         <v>6.4025901068999998E-3</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="41">
         <v>0.1369863013699</v>
       </c>
-      <c r="F17" s="43">
+      <c r="F17" s="41">
         <v>-4.6891825237000001E-3</v>
       </c>
-      <c r="H17" s="43">
+      <c r="H17" s="41">
         <v>0.1369863013699</v>
       </c>
-      <c r="I17" s="43">
+      <c r="I17" s="41">
         <v>-2.387301238E-4</v>
       </c>
-      <c r="K17" s="43">
+      <c r="K17" s="41">
         <v>5.0054794520548</v>
       </c>
-      <c r="L17" s="43">
+      <c r="L17" s="41">
         <v>0.113</v>
       </c>
-      <c r="N17" s="43">
+      <c r="N17" s="41">
         <v>1.6968820364574999</v>
       </c>
-      <c r="O17" s="43">
+      <c r="O17" s="41">
         <v>1.4215725085412001</v>
       </c>
-      <c r="P17" s="43">
+      <c r="P17" s="41">
         <v>1.1950129417736</v>
       </c>
-      <c r="Q17" s="43">
+      <c r="Q17" s="41">
         <v>1.0039245368603</v>
       </c>
-      <c r="R17" s="43">
+      <c r="R17" s="41">
         <v>0.84111859973860004</v>
       </c>
-      <c r="T17" s="43">
+      <c r="T17" s="41">
         <v>0.1207172875696</v>
       </c>
-      <c r="U17" s="43">
+      <c r="U17" s="41">
         <v>0.1144848812645</v>
       </c>
-      <c r="V17" s="43">
+      <c r="V17" s="41">
         <v>0.113</v>
       </c>
-      <c r="W17" s="43">
+      <c r="W17" s="41">
         <v>0.1169848812645</v>
       </c>
-      <c r="X17" s="43">
+      <c r="X17" s="41">
         <v>0.1249672875696</v>
       </c>
     </row>
     <row r="18" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B18" s="43">
+      <c r="B18" s="41">
         <v>0.1397260273973</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="41">
         <v>6.4035052759000002E-3</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="41">
         <v>0.1397260273973</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="41">
         <v>-4.6774571225E-3</v>
       </c>
-      <c r="H18" s="43">
+      <c r="H18" s="41">
         <v>0.1397260273973</v>
       </c>
-      <c r="I18" s="43">
+      <c r="I18" s="41">
         <v>-2.2195525230000001E-4</v>
       </c>
-      <c r="K18" s="43">
+      <c r="K18" s="41">
         <v>7.0027397260274</v>
       </c>
-      <c r="L18" s="43">
+      <c r="L18" s="41">
         <v>0.11600000000000001</v>
       </c>
-      <c r="N18" s="43">
+      <c r="N18" s="41">
         <v>1.9150657702731</v>
       </c>
-      <c r="O18" s="43">
+      <c r="O18" s="41">
         <v>1.5397760422144999</v>
       </c>
-      <c r="P18" s="43">
+      <c r="P18" s="41">
         <v>1.2453515907585</v>
       </c>
-      <c r="Q18" s="43">
+      <c r="Q18" s="41">
         <v>1.0090643204533001</v>
       </c>
-      <c r="R18" s="43">
+      <c r="R18" s="41">
         <v>0.81659865197680004</v>
       </c>
-      <c r="T18" s="43">
+      <c r="T18" s="41">
         <v>0.1247241553668</v>
       </c>
-      <c r="U18" s="43">
+      <c r="U18" s="41">
         <v>0.1179863847286</v>
       </c>
-      <c r="V18" s="43">
+      <c r="V18" s="41">
         <v>0.11600000000000001</v>
       </c>
-      <c r="W18" s="43">
+      <c r="W18" s="41">
         <v>0.1194863847286</v>
       </c>
-      <c r="X18" s="43">
+      <c r="X18" s="41">
         <v>0.12727415536680001</v>
       </c>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="43">
+      <c r="B19" s="41">
         <v>0.158904109589</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="41">
         <v>6.4090278471999997E-3</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E19" s="41">
         <v>0.158904109589</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="41">
         <v>-4.5432963116999996E-3</v>
       </c>
-      <c r="H19" s="43">
+      <c r="H19" s="41">
         <v>0.158904109589</v>
       </c>
-      <c r="I19" s="43">
+      <c r="I19" s="41">
         <v>-1.2803804629999999E-4</v>
       </c>
-      <c r="K19" s="43">
+      <c r="K19" s="41">
         <v>10.0082191780822</v>
       </c>
-      <c r="L19" s="43">
+      <c r="L19" s="41">
         <v>0.1275</v>
       </c>
-      <c r="N19" s="43">
+      <c r="N19" s="41">
         <v>2.3036276843243999</v>
       </c>
-      <c r="O19" s="43">
+      <c r="O19" s="41">
         <v>1.7497661519151</v>
       </c>
-      <c r="P19" s="43">
+      <c r="P19" s="41">
         <v>1.3320278121696001</v>
       </c>
-      <c r="Q19" s="43">
+      <c r="Q19" s="41">
         <v>1.0103622687225999</v>
       </c>
-      <c r="R19" s="43">
+      <c r="R19" s="41">
         <v>0.76428424729959998</v>
       </c>
-      <c r="T19" s="43">
+      <c r="T19" s="41">
         <v>0.13325857752119999</v>
       </c>
-      <c r="U19" s="43">
+      <c r="U19" s="41">
         <v>0.127711137502</v>
       </c>
-      <c r="V19" s="43">
+      <c r="V19" s="41">
         <v>0.1275</v>
       </c>
-      <c r="W19" s="43">
+      <c r="W19" s="41">
         <v>0.132711137502</v>
       </c>
-      <c r="X19" s="43">
+      <c r="X19" s="41">
         <v>0.1417585775212</v>
       </c>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B20" s="43">
+      <c r="B20" s="41">
         <v>0.16986301369859999</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="41">
         <v>6.4116237102000003E-3</v>
       </c>
-      <c r="E20" s="43">
+      <c r="E20" s="41">
         <v>0.16986301369859999</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20" s="41">
         <v>-4.4390044505E-3</v>
       </c>
-      <c r="H20" s="43">
+      <c r="H20" s="41">
         <v>0.16986301369859999</v>
       </c>
-      <c r="I20" s="43">
+      <c r="I20" s="41">
         <v>1.7571377759999999E-4</v>
       </c>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="43"/>
-      <c r="Q20" s="43"/>
-      <c r="R20" s="43"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="41"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
@@ -25537,31 +25537,31 @@
       <c r="X20" s="3"/>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B21" s="43">
+      <c r="B21" s="41">
         <v>0.21643835616439999</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C21" s="41">
         <v>6.4197234600000003E-3</v>
       </c>
-      <c r="E21" s="43">
+      <c r="E21" s="41">
         <v>0.21643835616439999</v>
       </c>
-      <c r="F21" s="43">
+      <c r="F21" s="41">
         <v>-4.3975027565999998E-3</v>
       </c>
-      <c r="H21" s="43">
+      <c r="H21" s="41">
         <v>0.21643835616439999</v>
       </c>
-      <c r="I21" s="43">
+      <c r="I21" s="41">
         <v>-2.410794918E-4</v>
       </c>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="N21" s="43"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="43"/>
-      <c r="R21" s="43"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
@@ -25569,31 +25569,31 @@
       <c r="X21" s="3"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B22" s="43">
+      <c r="B22" s="41">
         <v>0.24657534246580001</v>
       </c>
-      <c r="C22" s="43">
+      <c r="C22" s="41">
         <v>6.4213195190000001E-3</v>
       </c>
-      <c r="E22" s="43">
+      <c r="E22" s="41">
         <v>0.24657534246580001</v>
       </c>
-      <c r="F22" s="43">
+      <c r="F22" s="41">
         <v>-4.6300166569000004E-3</v>
       </c>
-      <c r="H22" s="43">
+      <c r="H22" s="41">
         <v>0.24657534246580001</v>
       </c>
-      <c r="I22" s="43">
+      <c r="I22" s="41">
         <v>3.2273683800000002E-5</v>
       </c>
-      <c r="K22" s="43"/>
-      <c r="L22" s="43"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="43"/>
-      <c r="Q22" s="43"/>
-      <c r="R22" s="43"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
+      <c r="Q22" s="41"/>
+      <c r="R22" s="41"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
@@ -25601,31 +25601,31 @@
       <c r="X22" s="3"/>
     </row>
     <row r="23" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B23" s="43">
+      <c r="B23" s="41">
         <v>0.2520547945205</v>
       </c>
-      <c r="C23" s="43">
+      <c r="C23" s="41">
         <v>6.4215687061000004E-3</v>
       </c>
-      <c r="E23" s="43">
+      <c r="E23" s="41">
         <v>0.2520547945205</v>
       </c>
-      <c r="F23" s="43">
+      <c r="F23" s="41">
         <v>-4.6848830586999997E-3</v>
       </c>
-      <c r="H23" s="43">
+      <c r="H23" s="41">
         <v>0.2520547945205</v>
       </c>
-      <c r="I23" s="43">
+      <c r="I23" s="41">
         <v>-2.7845678809999998E-4</v>
       </c>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="43"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="41"/>
+      <c r="R23" s="41"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
@@ -25633,31 +25633,31 @@
       <c r="X23" s="3"/>
     </row>
     <row r="24" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B24" s="43">
+      <c r="B24" s="41">
         <v>0.33972602739730001</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="41">
         <v>6.4244624915000001E-3</v>
       </c>
-      <c r="E24" s="43">
+      <c r="E24" s="41">
         <v>0.33972602739730001</v>
       </c>
-      <c r="F24" s="43">
+      <c r="F24" s="41">
         <v>-4.8383338076000001E-3</v>
       </c>
-      <c r="H24" s="43">
+      <c r="H24" s="41">
         <v>0.33972602739730001</v>
       </c>
-      <c r="I24" s="43">
+      <c r="I24" s="41">
         <v>1.6127856239999999E-4</v>
       </c>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="43"/>
-      <c r="R24" s="43"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="41"/>
+      <c r="R24" s="41"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
@@ -25665,31 +25665,31 @@
       <c r="X24" s="3"/>
     </row>
     <row r="25" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B25" s="43">
+      <c r="B25" s="41">
         <v>0.34520547945210001</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="41">
         <v>6.4245945491000003E-3</v>
       </c>
-      <c r="E25" s="43">
+      <c r="E25" s="41">
         <v>0.34520547945210001</v>
       </c>
-      <c r="F25" s="43">
+      <c r="F25" s="41">
         <v>-4.7394224145000004E-3</v>
       </c>
-      <c r="H25" s="43">
+      <c r="H25" s="41">
         <v>0.34520547945210001</v>
       </c>
-      <c r="I25" s="43">
+      <c r="I25" s="41">
         <v>1.650391319E-4</v>
       </c>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="43"/>
-      <c r="R25" s="43"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="41"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
@@ -25697,31 +25697,31 @@
       <c r="X25" s="3"/>
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B26" s="43">
+      <c r="B26" s="41">
         <v>0.35068493150680002</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="41">
         <v>6.4247224799999997E-3</v>
       </c>
-      <c r="E26" s="43">
+      <c r="E26" s="41">
         <v>0.35068493150680002</v>
       </c>
-      <c r="F26" s="43">
+      <c r="F26" s="41">
         <v>-4.6373802141999997E-3</v>
       </c>
-      <c r="H26" s="43">
+      <c r="H26" s="41">
         <v>0.35068493150680002</v>
       </c>
-      <c r="I26" s="43">
+      <c r="I26" s="41">
         <v>3.6396103399999997E-5</v>
       </c>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="43"/>
+      <c r="K26" s="41"/>
+      <c r="L26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="41"/>
+      <c r="Q26" s="41"/>
+      <c r="R26" s="41"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
@@ -25729,31 +25729,31 @@
       <c r="X26" s="3"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B27" s="43">
+      <c r="B27" s="41">
         <v>0.38630136986300001</v>
       </c>
-      <c r="C27" s="43">
+      <c r="C27" s="41">
         <v>6.4341935690000003E-3</v>
       </c>
-      <c r="E27" s="43">
+      <c r="E27" s="41">
         <v>0.38630136986300001</v>
       </c>
-      <c r="F27" s="43">
+      <c r="F27" s="41">
         <v>-5.0062809223000004E-3</v>
       </c>
-      <c r="H27" s="43">
+      <c r="H27" s="41">
         <v>0.38630136986300001</v>
       </c>
-      <c r="I27" s="43">
+      <c r="I27" s="41">
         <v>-6.6875080980000003E-4</v>
       </c>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="43"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="41"/>
+      <c r="R27" s="41"/>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
@@ -25761,1042 +25761,1042 @@
       <c r="X27" s="3"/>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B28" s="43">
+      <c r="B28" s="41">
         <v>0.38904109589039998</v>
       </c>
-      <c r="C28" s="43">
+      <c r="C28" s="41">
         <v>6.4348502858999996E-3</v>
       </c>
-      <c r="E28" s="43">
+      <c r="E28" s="41">
         <v>0.38904109589039998</v>
       </c>
-      <c r="F28" s="43">
+      <c r="F28" s="41">
         <v>-5.1421264015000002E-3</v>
       </c>
-      <c r="H28" s="43">
+      <c r="H28" s="41">
         <v>0.38904109589039998</v>
       </c>
-      <c r="I28" s="43">
+      <c r="I28" s="41">
         <v>-4.4697237919999998E-4</v>
       </c>
     </row>
     <row r="29" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B29" s="43">
+      <c r="B29" s="41">
         <v>0.41917808219180003</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="41">
         <v>6.4415075923999997E-3</v>
       </c>
-      <c r="E29" s="43">
+      <c r="E29" s="41">
         <v>0.41917808219180003</v>
       </c>
-      <c r="F29" s="43">
+      <c r="F29" s="41">
         <v>-5.3400809077999998E-3</v>
       </c>
-      <c r="H29" s="43">
+      <c r="H29" s="41">
         <v>0.41917808219180003</v>
       </c>
-      <c r="I29" s="43">
+      <c r="I29" s="41">
         <v>8.4563110899999995E-5</v>
       </c>
     </row>
     <row r="30" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B30" s="43">
+      <c r="B30" s="41">
         <v>0.46575342465750003</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30" s="41">
         <v>6.4501015700000001E-3</v>
       </c>
-      <c r="E30" s="43">
+      <c r="E30" s="41">
         <v>0.46575342465750003</v>
       </c>
-      <c r="F30" s="43">
+      <c r="F30" s="41">
         <v>-5.4351926277999996E-3</v>
       </c>
-      <c r="H30" s="43">
+      <c r="H30" s="41">
         <v>0.46575342465750003</v>
       </c>
-      <c r="I30" s="43">
+      <c r="I30" s="41">
         <v>-1.8521255959999999E-4</v>
       </c>
     </row>
     <row r="31" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B31" s="43">
+      <c r="B31" s="41">
         <v>0.49863013698629999</v>
       </c>
-      <c r="C31" s="43">
+      <c r="C31" s="41">
         <v>6.4669730066000001E-3</v>
       </c>
-      <c r="E31" s="43">
+      <c r="E31" s="41">
         <v>0.49863013698629999</v>
       </c>
-      <c r="F31" s="43">
+      <c r="F31" s="41">
         <v>-5.5688374037999996E-3</v>
       </c>
-      <c r="H31" s="43">
+      <c r="H31" s="41">
         <v>0.49863013698629999</v>
       </c>
-      <c r="I31" s="43">
+      <c r="I31" s="41">
         <v>4.6805431299999997E-5</v>
       </c>
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B32" s="43">
+      <c r="B32" s="41">
         <v>0.50410958904110004</v>
       </c>
-      <c r="C32" s="43">
+      <c r="C32" s="41">
         <v>6.4695709632999997E-3</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="41">
         <v>0.50410958904110004</v>
       </c>
-      <c r="F32" s="43">
+      <c r="F32" s="41">
         <v>-5.5525857990000003E-3</v>
       </c>
-      <c r="H32" s="43">
+      <c r="H32" s="41">
         <v>0.50410958904110004</v>
       </c>
-      <c r="I32" s="43">
+      <c r="I32" s="41">
         <v>-2.4588188700000001E-5</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="43">
+      <c r="B33" s="41">
         <v>0.61369863013699999</v>
       </c>
-      <c r="C33" s="43">
+      <c r="C33" s="41">
         <v>6.5117877601000001E-3</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="41">
         <v>0.61369863013699999</v>
       </c>
-      <c r="F33" s="43">
+      <c r="F33" s="41">
         <v>-4.9884041669E-3</v>
       </c>
-      <c r="H33" s="43">
+      <c r="H33" s="41">
         <v>0.61369863013699999</v>
       </c>
-      <c r="I33" s="43">
+      <c r="I33" s="41">
         <v>-7.6659210400000007E-5</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="43">
+      <c r="B34" s="41">
         <v>0.61917808219180004</v>
       </c>
-      <c r="C34" s="43">
+      <c r="C34" s="41">
         <v>6.5135063200000001E-3</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="41">
         <v>0.61917808219180004</v>
       </c>
-      <c r="F34" s="43">
+      <c r="F34" s="41">
         <v>-5.0939830290000002E-3</v>
       </c>
-      <c r="H34" s="43">
+      <c r="H34" s="41">
         <v>0.61917808219180004</v>
       </c>
-      <c r="I34" s="43">
+      <c r="I34" s="41">
         <v>-2.806874436E-4</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="43">
+      <c r="B35" s="41">
         <v>0.63835616438359999</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C35" s="41">
         <v>6.5257344392000002E-3</v>
       </c>
-      <c r="E35" s="43">
+      <c r="E35" s="41">
         <v>0.63835616438359999</v>
       </c>
-      <c r="F35" s="43">
+      <c r="F35" s="41">
         <v>-5.3506075015999997E-3</v>
       </c>
-      <c r="H35" s="43">
+      <c r="H35" s="41">
         <v>0.63835616438359999</v>
       </c>
-      <c r="I35" s="43">
+      <c r="I35" s="41">
         <v>-6.0652694000000001E-6</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="43">
+      <c r="B36" s="41">
         <v>0.64657534246579995</v>
       </c>
-      <c r="C36" s="43">
+      <c r="C36" s="41">
         <v>6.5307530014000002E-3</v>
       </c>
-      <c r="E36" s="43">
+      <c r="E36" s="41">
         <v>0.64657534246579995</v>
       </c>
-      <c r="F36" s="43">
+      <c r="F36" s="41">
         <v>-5.292338154E-3</v>
       </c>
-      <c r="H36" s="43">
+      <c r="H36" s="41">
         <v>0.64657534246579995</v>
       </c>
-      <c r="I36" s="43">
+      <c r="I36" s="41">
         <v>5.1589089099999999E-5</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="43">
+      <c r="B37" s="41">
         <v>0.73424657534250004</v>
       </c>
-      <c r="C37" s="43">
+      <c r="C37" s="41">
         <v>6.5772933000000002E-3</v>
       </c>
-      <c r="E37" s="43">
+      <c r="E37" s="41">
         <v>0.73424657534250004</v>
       </c>
-      <c r="F37" s="43">
+      <c r="F37" s="41">
         <v>-5.9176800741000003E-3</v>
       </c>
-      <c r="H37" s="43">
+      <c r="H37" s="41">
         <v>0.73424657534250004</v>
       </c>
-      <c r="I37" s="43">
+      <c r="I37" s="41">
         <v>-1.6174401870000001E-4</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="43">
+      <c r="B38" s="41">
         <v>0.75068493150680005</v>
       </c>
-      <c r="C38" s="43">
+      <c r="C38" s="41">
         <v>6.5892403784000003E-3</v>
       </c>
-      <c r="E38" s="43">
+      <c r="E38" s="41">
         <v>0.75068493150680005</v>
       </c>
-      <c r="F38" s="43">
+      <c r="F38" s="41">
         <v>-6.0219444737999997E-3</v>
       </c>
-      <c r="H38" s="43">
+      <c r="H38" s="41">
         <v>0.75068493150680005</v>
       </c>
-      <c r="I38" s="43">
+      <c r="I38" s="41">
         <v>-1.028467048E-4</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="43">
+      <c r="B39" s="41">
         <v>0.76164383561640003</v>
       </c>
-      <c r="C39" s="43">
+      <c r="C39" s="41">
         <v>6.5969185965999997E-3</v>
       </c>
-      <c r="E39" s="43">
+      <c r="E39" s="41">
         <v>0.76164383561640003</v>
       </c>
-      <c r="F39" s="43">
+      <c r="F39" s="41">
         <v>-6.0423712763999996E-3</v>
       </c>
-      <c r="H39" s="43">
+      <c r="H39" s="41">
         <v>0.76164383561640003</v>
       </c>
-      <c r="I39" s="43">
+      <c r="I39" s="41">
         <v>2.0836517799999999E-5</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="43">
+      <c r="B40" s="41">
         <v>0.84931506849320004</v>
       </c>
-      <c r="C40" s="43">
+      <c r="C40" s="41">
         <v>6.6512110299999996E-3</v>
       </c>
-      <c r="E40" s="43">
+      <c r="E40" s="41">
         <v>0.84931506849320004</v>
       </c>
-      <c r="F40" s="43">
+      <c r="F40" s="41">
         <v>-5.8833015775999996E-3</v>
       </c>
-      <c r="H40" s="43">
+      <c r="H40" s="41">
         <v>0.84931506849320004</v>
       </c>
-      <c r="I40" s="43">
+      <c r="I40" s="41">
         <v>-2.4290283649999999E-4</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="43">
+      <c r="B41" s="41">
         <v>0.86301369863010002</v>
       </c>
-      <c r="C41" s="43">
+      <c r="C41" s="41">
         <v>6.6630146359000003E-3</v>
       </c>
-      <c r="E41" s="43">
+      <c r="E41" s="41">
         <v>0.86301369863010002</v>
       </c>
-      <c r="F41" s="43">
+      <c r="F41" s="41">
         <v>-6.1040126534999996E-3</v>
       </c>
-      <c r="H41" s="43">
+      <c r="H41" s="41">
         <v>0.86301369863010002</v>
       </c>
-      <c r="I41" s="43">
+      <c r="I41" s="41">
         <v>-1.1504406560000001E-4</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="43">
+      <c r="B42" s="41">
         <v>0.88767123287670002</v>
       </c>
-      <c r="C42" s="43">
+      <c r="C42" s="41">
         <v>6.6833430681999999E-3</v>
       </c>
-      <c r="E42" s="43">
+      <c r="E42" s="41">
         <v>0.88767123287670002</v>
       </c>
-      <c r="F42" s="43">
+      <c r="F42" s="41">
         <v>-6.7739739283000002E-3</v>
       </c>
-      <c r="H42" s="43">
+      <c r="H42" s="41">
         <v>0.88767123287670002</v>
       </c>
-      <c r="I42" s="43">
+      <c r="I42" s="41">
         <v>-3.6385621630000001E-4</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="43">
+      <c r="B43" s="41">
         <v>0.89589041095889999</v>
       </c>
-      <c r="C43" s="43">
+      <c r="C43" s="41">
         <v>6.6898705465000003E-3</v>
       </c>
-      <c r="E43" s="43">
+      <c r="E43" s="41">
         <v>0.89589041095889999</v>
       </c>
-      <c r="F43" s="43">
+      <c r="F43" s="41">
         <v>-6.9789350129E-3</v>
       </c>
-      <c r="H43" s="43">
+      <c r="H43" s="41">
         <v>0.89589041095889999</v>
       </c>
-      <c r="I43" s="43">
+      <c r="I43" s="41">
         <v>-1.3705592610000001E-4</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="43">
+      <c r="B44" s="41">
         <v>1</v>
       </c>
-      <c r="C44" s="43">
+      <c r="C44" s="41">
         <v>6.7632644391E-3</v>
       </c>
-      <c r="E44" s="43">
+      <c r="E44" s="41">
         <v>1</v>
       </c>
-      <c r="F44" s="43">
+      <c r="F44" s="41">
         <v>-6.8277489972000003E-3</v>
       </c>
-      <c r="H44" s="43">
+      <c r="H44" s="41">
         <v>1</v>
       </c>
-      <c r="I44" s="43">
+      <c r="I44" s="41">
         <v>9.86268326E-5</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="43">
+      <c r="B45" s="41">
         <v>1.0109589041096001</v>
       </c>
-      <c r="C45" s="43">
+      <c r="C45" s="41">
         <v>6.7701107671E-3</v>
       </c>
-      <c r="E45" s="43">
+      <c r="E45" s="41">
         <v>1.0109589041096001</v>
       </c>
-      <c r="F45" s="43">
+      <c r="F45" s="41">
         <v>-6.6575289305000002E-3</v>
       </c>
-      <c r="H45" s="43">
+      <c r="H45" s="41">
         <v>1.0109589041096001</v>
       </c>
-      <c r="I45" s="43">
+      <c r="I45" s="41">
         <v>8.87202968E-5</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="43">
+      <c r="B46" s="41">
         <v>1.0164383561643999</v>
       </c>
-      <c r="C46" s="43">
+      <c r="C46" s="41">
         <v>6.7734785699999998E-3</v>
       </c>
-      <c r="E46" s="43">
+      <c r="E46" s="41">
         <v>1.0164383561643999</v>
       </c>
-      <c r="F46" s="43">
+      <c r="F46" s="41">
         <v>-6.5746055189000001E-3</v>
       </c>
-      <c r="H46" s="43">
+      <c r="H46" s="41">
         <v>1.0164383561643999</v>
       </c>
-      <c r="I46" s="43">
+      <c r="I46" s="41">
         <v>8.5471060699999994E-5</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="43">
+      <c r="B47" s="41">
         <v>1.2630136986300999</v>
       </c>
-      <c r="C47" s="43">
+      <c r="C47" s="41">
         <v>6.9809357000000004E-3</v>
       </c>
-      <c r="E47" s="43">
+      <c r="E47" s="41">
         <v>1.2630136986300999</v>
       </c>
-      <c r="F47" s="43">
+      <c r="F47" s="41">
         <v>-4.3576966562999999E-3</v>
       </c>
-      <c r="H47" s="43">
+      <c r="H47" s="41">
         <v>1.2630136986300999</v>
       </c>
-      <c r="I47" s="43">
+      <c r="I47" s="41">
         <v>3.5723856600000001E-5</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="43">
+      <c r="B48" s="41">
         <v>1.5150684931506999</v>
       </c>
-      <c r="C48" s="43">
+      <c r="C48" s="41">
         <v>7.2172558099999999E-3</v>
       </c>
-      <c r="E48" s="43">
+      <c r="E48" s="41">
         <v>1.5150684931506999</v>
       </c>
-      <c r="F48" s="43">
+      <c r="F48" s="41">
         <v>-3.8549288913999999E-3</v>
       </c>
-      <c r="H48" s="43">
+      <c r="H48" s="41">
         <v>1.5150684931506999</v>
       </c>
-      <c r="I48" s="43">
+      <c r="I48" s="41">
         <v>9.7648731999999997E-6</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="43">
+      <c r="B49" s="41">
         <v>1.7643835616437999</v>
       </c>
-      <c r="C49" s="43">
+      <c r="C49" s="41">
         <v>7.46919165E-3</v>
       </c>
-      <c r="E49" s="43">
+      <c r="E49" s="41">
         <v>1.7643835616437999</v>
       </c>
-      <c r="F49" s="43">
+      <c r="F49" s="41">
         <v>-4.0126723517E-3</v>
       </c>
-      <c r="H49" s="43">
+      <c r="H49" s="41">
         <v>1.7643835616437999</v>
       </c>
-      <c r="I49" s="43">
+      <c r="I49" s="41">
         <v>-6.9889569999999996E-7</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="43">
+      <c r="B50" s="41">
         <v>1.9972602739726</v>
       </c>
-      <c r="C50" s="43">
+      <c r="C50" s="41">
         <v>7.7177879162999997E-3</v>
       </c>
-      <c r="E50" s="43">
+      <c r="E50" s="41">
         <v>1.9972602739726</v>
       </c>
-      <c r="F50" s="43">
+      <c r="F50" s="41">
         <v>-4.2358605934000003E-3</v>
       </c>
-      <c r="H50" s="43">
+      <c r="H50" s="41">
         <v>1.9972602739726</v>
       </c>
-      <c r="I50" s="43">
+      <c r="I50" s="41">
         <v>-4.5267232200000003E-5</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="43">
+      <c r="B51" s="41">
         <v>2.0082191780822001</v>
       </c>
-      <c r="C51" s="43">
+      <c r="C51" s="41">
         <v>7.7297740676000003E-3</v>
       </c>
-      <c r="E51" s="43">
+      <c r="E51" s="41">
         <v>2.0082191780822001</v>
       </c>
-      <c r="F51" s="43">
+      <c r="F51" s="41">
         <v>-4.2446973020000001E-3</v>
       </c>
-      <c r="H51" s="43">
+      <c r="H51" s="41">
         <v>2.0082191780822001</v>
       </c>
-      <c r="I51" s="43">
+      <c r="I51" s="41">
         <v>-3.1501870000000002E-7</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="43">
+      <c r="B52" s="41">
         <v>2.0136986301370001</v>
       </c>
-      <c r="C52" s="43">
+      <c r="C52" s="41">
         <v>7.7357759799999998E-3</v>
       </c>
-      <c r="E52" s="43">
+      <c r="E52" s="41">
         <v>2.0136986301370001</v>
       </c>
-      <c r="F52" s="43">
+      <c r="F52" s="41">
         <v>-4.2473483202999998E-3</v>
       </c>
-      <c r="H52" s="43">
+      <c r="H52" s="41">
         <v>2.0136986301370001</v>
       </c>
-      <c r="I52" s="43">
+      <c r="I52" s="41">
         <v>1.3402516000000001E-6</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="43">
+      <c r="B53" s="41">
         <v>2.9972602739726</v>
       </c>
-      <c r="C53" s="43">
+      <c r="C53" s="41">
         <v>8.8854232401000006E-3</v>
       </c>
-      <c r="E53" s="43">
+      <c r="E53" s="41">
         <v>2.9972602739726</v>
       </c>
-      <c r="F53" s="43">
+      <c r="F53" s="41">
         <v>-3.8447712597000001E-3</v>
       </c>
-      <c r="H53" s="43">
+      <c r="H53" s="41">
         <v>2.9972602739726</v>
       </c>
-      <c r="I53" s="43">
+      <c r="I53" s="41">
         <v>-2.7958050300000001E-5</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="43">
+      <c r="B54" s="41">
         <v>3.0082191780822001</v>
       </c>
-      <c r="C54" s="43">
+      <c r="C54" s="41">
         <v>8.8988703530000005E-3</v>
       </c>
-      <c r="E54" s="43">
+      <c r="E54" s="41">
         <v>3.0082191780822001</v>
       </c>
-      <c r="F54" s="43">
+      <c r="F54" s="41">
         <v>-3.8401977962000001E-3</v>
       </c>
-      <c r="H54" s="43">
+      <c r="H54" s="41">
         <v>3.0082191780822001</v>
       </c>
-      <c r="I54" s="43">
+      <c r="I54" s="41">
         <v>1.3225377E-6</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="43">
+      <c r="B55" s="41">
         <v>3.0136986301370001</v>
       </c>
-      <c r="C55" s="43">
+      <c r="C55" s="41">
         <v>8.9055982300000006E-3</v>
       </c>
-      <c r="E55" s="43">
+      <c r="E55" s="41">
         <v>3.0136986301370001</v>
       </c>
-      <c r="F55" s="43">
+      <c r="F55" s="41">
         <v>-3.8363314240000002E-3</v>
       </c>
-      <c r="H55" s="43">
+      <c r="H55" s="41">
         <v>3.0136986301370001</v>
       </c>
-      <c r="I55" s="43">
+      <c r="I55" s="41">
         <v>-3.3861605999999998E-5</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="43">
+      <c r="B56" s="41">
         <v>4.0082191780822001</v>
       </c>
-      <c r="C56" s="43">
+      <c r="C56" s="41">
         <v>1.0149245695399999E-2</v>
       </c>
-      <c r="E56" s="43">
+      <c r="E56" s="41">
         <v>4.0082191780822001</v>
       </c>
-      <c r="F56" s="43">
+      <c r="F56" s="41">
         <v>-3.0420596103999998E-3</v>
       </c>
-      <c r="H56" s="43">
+      <c r="H56" s="41">
         <v>4.0082191780822001</v>
       </c>
-      <c r="I56" s="43">
+      <c r="I56" s="41">
         <v>3.4760200000000002E-7</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="43">
+      <c r="B57" s="41">
         <v>4.0136986301370001</v>
       </c>
-      <c r="C57" s="43">
+      <c r="C57" s="41">
         <v>1.0156116539999999E-2</v>
       </c>
-      <c r="E57" s="43">
+      <c r="E57" s="41">
         <v>4.0136986301370001</v>
       </c>
-      <c r="F57" s="43">
+      <c r="F57" s="41">
         <v>-3.0373640461999999E-3</v>
       </c>
-      <c r="H57" s="43">
+      <c r="H57" s="41">
         <v>4.0136986301370001</v>
       </c>
-      <c r="I57" s="43">
+      <c r="I57" s="41">
         <v>-1.9807499500000002E-5</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="43">
+      <c r="B58" s="41">
         <v>5.0054794520548</v>
       </c>
-      <c r="C58" s="43">
+      <c r="C58" s="41">
         <v>1.13947054096E-2</v>
       </c>
-      <c r="E58" s="43">
+      <c r="E58" s="41">
         <v>5.0054794520548</v>
       </c>
-      <c r="F58" s="43">
+      <c r="F58" s="41">
         <v>-2.0140472746999999E-3</v>
       </c>
-      <c r="H58" s="43">
+      <c r="H58" s="41">
         <v>5.0054794520548</v>
       </c>
-      <c r="I58" s="43">
+      <c r="I58" s="41">
         <v>1.2203675000000001E-6</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="43">
+      <c r="B59" s="41">
         <v>5.0109589041096001</v>
       </c>
-      <c r="C59" s="43">
+      <c r="C59" s="41">
         <v>1.14015468086E-2</v>
       </c>
-      <c r="E59" s="43">
+      <c r="E59" s="41">
         <v>5.0109589041096001</v>
       </c>
-      <c r="F59" s="43">
+      <c r="F59" s="41">
         <v>-2.0077694739999998E-3</v>
       </c>
-      <c r="H59" s="43">
+      <c r="H59" s="41">
         <v>5.0109589041096001</v>
       </c>
-      <c r="I59" s="43">
+      <c r="I59" s="41">
         <v>-1.3999513099999999E-5</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="43">
+      <c r="B60" s="41">
         <v>5.0246575342466002</v>
       </c>
-      <c r="C60" s="43">
+      <c r="C60" s="41">
         <v>1.1418651239999999E-2</v>
       </c>
-      <c r="E60" s="43">
+      <c r="E60" s="41">
         <v>5.0246575342466002</v>
       </c>
-      <c r="F60" s="43">
+      <c r="F60" s="41">
         <v>-1.9920578539E-3</v>
       </c>
-      <c r="H60" s="43">
+      <c r="H60" s="41">
         <v>5.0246575342466002</v>
       </c>
-      <c r="I60" s="43">
+      <c r="I60" s="41">
         <v>1.2243287E-6</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="43">
+      <c r="B61" s="41">
         <v>6.0219178082192002</v>
       </c>
-      <c r="C61" s="43">
+      <c r="C61" s="41">
         <v>1.264840423E-2</v>
       </c>
-      <c r="E61" s="43">
+      <c r="E61" s="41">
         <v>6.0219178082192002</v>
       </c>
-      <c r="F61" s="43">
+      <c r="F61" s="41">
         <v>-7.8795282479999997E-4</v>
       </c>
-      <c r="H61" s="43">
+      <c r="H61" s="41">
         <v>6.0219178082192002</v>
       </c>
-      <c r="I61" s="43">
+      <c r="I61" s="41">
         <v>1.7979840999999999E-6</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="43">
+      <c r="B62" s="41">
         <v>7.0027397260274</v>
       </c>
-      <c r="C62" s="43">
+      <c r="C62" s="41">
         <v>1.3786018799899999E-2</v>
       </c>
-      <c r="E62" s="43">
+      <c r="E62" s="41">
         <v>7.0027397260274</v>
       </c>
-      <c r="F62" s="43">
+      <c r="F62" s="41">
         <v>4.8176653209999997E-4</v>
       </c>
-      <c r="H62" s="43">
+      <c r="H62" s="41">
         <v>7.0027397260274</v>
       </c>
-      <c r="I62" s="43">
+      <c r="I62" s="41">
         <v>-6.9743163999999996E-6</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="43">
+      <c r="B63" s="41">
         <v>7.0136986301370001</v>
       </c>
-      <c r="C63" s="43">
+      <c r="C63" s="41">
         <v>1.37982907523E-2</v>
       </c>
-      <c r="E63" s="43">
+      <c r="E63" s="41">
         <v>7.0136986301370001</v>
       </c>
-      <c r="F63" s="43">
+      <c r="F63" s="41">
         <v>4.9611376510000002E-4</v>
       </c>
-      <c r="H63" s="43">
+      <c r="H63" s="41">
         <v>7.0136986301370001</v>
       </c>
-      <c r="I63" s="43">
+      <c r="I63" s="41">
         <v>2.3987668000000001E-6</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="43">
+      <c r="B64" s="41">
         <v>7.0191780821918002</v>
       </c>
-      <c r="C64" s="43">
+      <c r="C64" s="41">
         <v>1.380442326E-2</v>
       </c>
-      <c r="E64" s="43">
+      <c r="E64" s="41">
         <v>7.0191780821918002</v>
       </c>
-      <c r="F64" s="43">
+      <c r="F64" s="41">
         <v>5.0328735750000003E-4</v>
       </c>
-      <c r="H64" s="43">
+      <c r="H64" s="41">
         <v>7.0191780821918002</v>
       </c>
-      <c r="I64" s="43">
+      <c r="I64" s="41">
         <v>2.4007969000000001E-6</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B65" s="43">
+      <c r="B65" s="41">
         <v>8.0164383561644001</v>
       </c>
-      <c r="C65" s="43">
+      <c r="C65" s="41">
         <v>1.4880430300000001E-2</v>
       </c>
-      <c r="E65" s="43">
+      <c r="E65" s="41">
         <v>8.0164383561644001</v>
       </c>
-      <c r="F65" s="43">
+      <c r="F65" s="41">
         <v>1.7981620868E-3</v>
       </c>
-      <c r="H65" s="43">
+      <c r="H65" s="41">
         <v>8.0164383561644001</v>
       </c>
-      <c r="I65" s="43">
+      <c r="I65" s="41">
         <v>2.6608752E-6</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B66" s="43">
+      <c r="B66" s="41">
         <v>9.0191780821918002</v>
       </c>
-      <c r="C66" s="43">
+      <c r="C66" s="41">
         <v>1.5873413940000001E-2</v>
       </c>
-      <c r="E66" s="43">
+      <c r="E66" s="41">
         <v>9.0191780821918002</v>
       </c>
-      <c r="F66" s="43">
+      <c r="F66" s="41">
         <v>3.0369365098999999E-3</v>
       </c>
-      <c r="H66" s="43">
+      <c r="H66" s="41">
         <v>9.0191780821918002</v>
       </c>
-      <c r="I66" s="43">
+      <c r="I66" s="41">
         <v>-3.8421239999999998E-6</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" s="43">
+      <c r="B67" s="41">
         <v>10.0082191780822</v>
       </c>
-      <c r="C67" s="43">
+      <c r="C67" s="41">
         <v>1.6754918943800001E-2</v>
       </c>
-      <c r="E67" s="43">
+      <c r="E67" s="41">
         <v>10.0082191780822</v>
       </c>
-      <c r="F67" s="43">
+      <c r="F67" s="41">
         <v>4.1362766215000003E-3</v>
       </c>
-      <c r="H67" s="43">
+      <c r="H67" s="41">
         <v>10.0082191780822</v>
       </c>
-      <c r="I67" s="43">
+      <c r="I67" s="41">
         <v>2.4127046E-6</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B68" s="43">
+      <c r="B68" s="41">
         <v>10.013698630137</v>
       </c>
-      <c r="C68" s="43">
+      <c r="C68" s="41">
         <v>1.6759567579E-2</v>
       </c>
-      <c r="E68" s="43">
+      <c r="E68" s="41">
         <v>10.013698630137</v>
       </c>
-      <c r="F68" s="43">
+      <c r="F68" s="41">
         <v>4.1420122488000002E-3</v>
       </c>
-      <c r="H68" s="43">
+      <c r="H68" s="41">
         <v>10.013698630137</v>
       </c>
-      <c r="I68" s="43">
+      <c r="I68" s="41">
         <v>-6.3167837999999999E-6</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" s="43">
+      <c r="B69" s="41">
         <v>10.027397260274</v>
       </c>
-      <c r="C69" s="43">
+      <c r="C69" s="41">
         <v>1.6771179109999999E-2</v>
       </c>
-      <c r="E69" s="43">
+      <c r="E69" s="41">
         <v>10.027397260274</v>
       </c>
-      <c r="F69" s="43">
+      <c r="F69" s="41">
         <v>4.1563347071000003E-3</v>
       </c>
-      <c r="H69" s="43">
+      <c r="H69" s="41">
         <v>10.027397260274</v>
       </c>
-      <c r="I69" s="43">
+      <c r="I69" s="41">
         <v>2.4069873000000001E-6</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B70" s="43">
+      <c r="B70" s="41">
         <v>12.0246575342466</v>
       </c>
-      <c r="C70" s="43">
+      <c r="C70" s="41">
         <v>1.8301476769999998E-2</v>
       </c>
-      <c r="E70" s="43">
+      <c r="E70" s="41">
         <v>12.0246575342466</v>
       </c>
-      <c r="F70" s="43">
+      <c r="F70" s="41">
         <v>5.9841452153999997E-3</v>
       </c>
-      <c r="H70" s="43">
+      <c r="H70" s="41">
         <v>12.0246575342466</v>
       </c>
-      <c r="I70" s="43">
+      <c r="I70" s="41">
         <v>1.8319129E-6</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B71" s="43">
+      <c r="B71" s="41">
         <v>15.0164383561644</v>
       </c>
-      <c r="C71" s="43">
+      <c r="C71" s="41">
         <v>1.99887654406E-2</v>
       </c>
-      <c r="E71" s="43">
+      <c r="E71" s="41">
         <v>15.0164383561644</v>
       </c>
-      <c r="F71" s="43">
+      <c r="F71" s="41">
         <v>7.8839890558999991E-3</v>
       </c>
-      <c r="H71" s="43">
+      <c r="H71" s="41">
         <v>15.0164383561644</v>
       </c>
-      <c r="I71" s="43">
+      <c r="I71" s="41">
         <v>1.2807922999999999E-6</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" s="43">
+      <c r="B72" s="41">
         <v>15.0219178082192</v>
       </c>
-      <c r="C72" s="43">
+      <c r="C72" s="41">
         <v>1.9991276459999999E-2</v>
       </c>
-      <c r="E72" s="43">
+      <c r="E72" s="41">
         <v>15.0219178082192</v>
       </c>
-      <c r="F72" s="43">
+      <c r="F72" s="41">
         <v>7.8867101130999998E-3</v>
       </c>
-      <c r="H72" s="43">
+      <c r="H72" s="41">
         <v>15.0219178082192</v>
       </c>
-      <c r="I72" s="43">
+      <c r="I72" s="41">
         <v>-2.9263192E-6</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" s="43">
+      <c r="B73" s="41">
         <v>20.0191780821918</v>
       </c>
-      <c r="C73" s="43">
+      <c r="C73" s="41">
         <v>2.1624072629099999E-2</v>
       </c>
-      <c r="E73" s="43">
+      <c r="E73" s="41">
         <v>20.0191780821918</v>
       </c>
-      <c r="F73" s="43">
+      <c r="F73" s="41">
         <v>9.5551154085000006E-3</v>
       </c>
-      <c r="H73" s="43">
+      <c r="H73" s="41">
         <v>20.0191780821918</v>
       </c>
-      <c r="I73" s="43">
+      <c r="I73" s="41">
         <v>7.5349260000000001E-7</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B74" s="43">
+      <c r="B74" s="41">
         <v>20.0246575342466</v>
       </c>
-      <c r="C74" s="43">
+      <c r="C74" s="41">
         <v>2.1625262249999999E-2</v>
       </c>
-      <c r="E74" s="43">
+      <c r="E74" s="41">
         <v>20.0246575342466</v>
       </c>
-      <c r="F74" s="43">
+      <c r="F74" s="41">
         <v>9.5562456159000008E-3</v>
       </c>
-      <c r="H74" s="43">
+      <c r="H74" s="41">
         <v>20.0246575342466</v>
       </c>
-      <c r="I74" s="43">
+      <c r="I74" s="41">
         <v>-2.6090055E-6</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" s="43">
+      <c r="B75" s="41">
         <v>25.0301369863014</v>
       </c>
-      <c r="C75" s="43">
+      <c r="C75" s="41">
         <v>2.233253889E-2</v>
       </c>
-      <c r="E75" s="43">
+      <c r="E75" s="41">
         <v>25.0301369863014</v>
       </c>
-      <c r="F75" s="43">
+      <c r="F75" s="41">
         <v>1.0201579468899999E-2</v>
       </c>
-      <c r="H75" s="43">
+      <c r="H75" s="41">
         <v>25.0301369863014</v>
       </c>
-      <c r="I75" s="43">
+      <c r="I75" s="41">
         <v>-2.1142105999999999E-6</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B76" s="43">
+      <c r="B76" s="41">
         <v>30.027397260274</v>
       </c>
-      <c r="C76" s="43">
+      <c r="C76" s="41">
         <v>2.2527480838600001E-2</v>
       </c>
-      <c r="E76" s="43">
+      <c r="E76" s="41">
         <v>30.027397260274</v>
       </c>
-      <c r="F76" s="43">
+      <c r="F76" s="41">
         <v>1.03949678881E-2</v>
       </c>
-      <c r="H76" s="43">
+      <c r="H76" s="41">
         <v>30.027397260274</v>
       </c>
-      <c r="I76" s="43">
+      <c r="I76" s="41">
         <v>6.5530229999999998E-7</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" s="43">
+      <c r="B77" s="41">
         <v>30.0328767123288</v>
       </c>
-      <c r="C77" s="43">
+      <c r="C77" s="41">
         <v>2.2527515929999999E-2</v>
       </c>
-      <c r="E77" s="43">
+      <c r="E77" s="41">
         <v>30.0328767123288</v>
       </c>
-      <c r="F77" s="43">
+      <c r="F77" s="41">
         <v>1.0395127883700001E-2</v>
       </c>
-      <c r="H77" s="43">
+      <c r="H77" s="41">
         <v>30.0328767123288</v>
       </c>
-      <c r="I77" s="43">
+      <c r="I77" s="41">
         <v>6.5531090000000004E-7</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" s="43">
+      <c r="B78" s="41">
         <v>40.0438356164384</v>
       </c>
-      <c r="C78" s="43">
+      <c r="C78" s="41">
         <v>2.2212955789999999E-2</v>
       </c>
-      <c r="E78" s="43">
+      <c r="E78" s="41">
         <v>40.0438356164384</v>
       </c>
-      <c r="F78" s="43">
+      <c r="F78" s="41">
         <v>1.04285935224E-2</v>
       </c>
-      <c r="H78" s="43">
+      <c r="H78" s="41">
         <v>40.0438356164384</v>
       </c>
-      <c r="I78" s="43">
+      <c r="I78" s="41">
         <v>6.940074E-7</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B79" s="43">
+      <c r="B79" s="41">
         <v>50.0520547945206</v>
       </c>
-      <c r="C79" s="43">
+      <c r="C79" s="41">
         <v>2.1560213200000001E-2</v>
       </c>
-      <c r="E79" s="43">
+      <c r="E79" s="41">
         <v>50.0520547945206</v>
       </c>
-      <c r="F79" s="43">
+      <c r="F79" s="41">
         <v>1.0250870251000001E-2</v>
       </c>
-      <c r="H79" s="43">
+      <c r="H79" s="41">
         <v>50.0520547945206</v>
       </c>
-      <c r="I79" s="43">
+      <c r="I79" s="41">
         <v>4.080034E-7</v>
       </c>
     </row>
@@ -30879,7 +30879,7 @@
       </c>
     </row>
     <row r="96" spans="1:253" x14ac:dyDescent="0.25">
-      <c r="B96" s="41">
+      <c r="B96" s="42">
         <v>1</v>
       </c>
       <c r="C96" s="24" t="s">
@@ -31331,7 +31331,7 @@
       <c r="IS96" s="18"/>
     </row>
     <row r="97" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B97" s="41"/>
+      <c r="B97" s="42"/>
       <c r="C97" s="24" t="s">
         <v>37</v>
       </c>
@@ -31781,7 +31781,7 @@
       <c r="IS97" s="26"/>
     </row>
     <row r="98" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B98" s="41">
+      <c r="B98" s="42">
         <v>2</v>
       </c>
       <c r="C98" s="24" t="s">
@@ -32233,7 +32233,7 @@
       <c r="IS98" s="18"/>
     </row>
     <row r="99" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B99" s="41"/>
+      <c r="B99" s="42"/>
       <c r="C99" s="24" t="s">
         <v>37</v>
       </c>
@@ -32683,7 +32683,7 @@
       <c r="IS99" s="26"/>
     </row>
     <row r="100" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B100" s="41">
+      <c r="B100" s="42">
         <v>3</v>
       </c>
       <c r="C100" s="24" t="s">
@@ -33075,7 +33075,7 @@
       <c r="IS100" s="18"/>
     </row>
     <row r="101" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B101" s="41"/>
+      <c r="B101" s="42"/>
       <c r="C101" s="24" t="s">
         <v>37</v>
       </c>
@@ -33465,7 +33465,7 @@
       <c r="IS101" s="26"/>
     </row>
     <row r="102" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B102" s="41">
+      <c r="B102" s="42">
         <v>4</v>
       </c>
       <c r="C102" s="24" t="s">
@@ -33869,7 +33869,7 @@
       <c r="IS102" s="18"/>
     </row>
     <row r="103" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B103" s="41"/>
+      <c r="B103" s="42"/>
       <c r="C103" s="24" t="s">
         <v>37</v>
       </c>
@@ -34271,7 +34271,7 @@
       <c r="IS103" s="26"/>
     </row>
     <row r="104" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B104" s="41">
+      <c r="B104" s="42">
         <v>5</v>
       </c>
       <c r="C104" s="24" t="s">
@@ -34687,7 +34687,7 @@
       <c r="IS104" s="18"/>
     </row>
     <row r="105" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B105" s="41"/>
+      <c r="B105" s="42"/>
       <c r="C105" s="24" t="s">
         <v>37</v>
       </c>
@@ -35101,7 +35101,7 @@
       <c r="IS105" s="26"/>
     </row>
     <row r="106" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B106" s="41">
+      <c r="B106" s="42">
         <v>6</v>
       </c>
       <c r="C106" s="24" t="s">
@@ -35485,7 +35485,7 @@
       <c r="IS106" s="18"/>
     </row>
     <row r="107" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B107" s="41"/>
+      <c r="B107" s="42"/>
       <c r="C107" s="24" t="s">
         <v>37</v>
       </c>
@@ -35867,7 +35867,7 @@
       <c r="IS107" s="26"/>
     </row>
     <row r="108" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B108" s="41">
+      <c r="B108" s="42">
         <v>7</v>
       </c>
       <c r="C108" s="24" t="s">
@@ -36267,7 +36267,7 @@
       <c r="IS108" s="18"/>
     </row>
     <row r="109" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B109" s="41"/>
+      <c r="B109" s="42"/>
       <c r="C109" s="24" t="s">
         <v>37</v>
       </c>
@@ -36665,7 +36665,7 @@
       <c r="IS109" s="26"/>
     </row>
     <row r="110" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B110" s="41">
+      <c r="B110" s="42">
         <v>8</v>
       </c>
       <c r="C110" s="24" t="s">
@@ -37057,7 +37057,7 @@
       <c r="IS110" s="18"/>
     </row>
     <row r="111" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B111" s="41"/>
+      <c r="B111" s="42"/>
       <c r="C111" s="24" t="s">
         <v>37</v>
       </c>
@@ -37447,7 +37447,7 @@
       <c r="IS111" s="26"/>
     </row>
     <row r="112" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B112" s="41">
+      <c r="B112" s="42">
         <v>9</v>
       </c>
       <c r="C112" s="24" t="s">
@@ -37859,7 +37859,7 @@
       <c r="IS112" s="18"/>
     </row>
     <row r="113" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B113" s="41"/>
+      <c r="B113" s="42"/>
       <c r="C113" s="24" t="s">
         <v>37</v>
       </c>
@@ -38269,7 +38269,7 @@
       <c r="IS113" s="26"/>
     </row>
     <row r="114" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B114" s="41">
+      <c r="B114" s="42">
         <v>10</v>
       </c>
       <c r="C114" s="24" t="s">
@@ -38741,7 +38741,7 @@
       <c r="IS114" s="18"/>
     </row>
     <row r="115" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B115" s="41"/>
+      <c r="B115" s="42"/>
       <c r="C115" s="24" t="s">
         <v>37</v>
       </c>
@@ -39211,7 +39211,7 @@
       <c r="IS115" s="26"/>
     </row>
     <row r="116" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B116" s="41">
+      <c r="B116" s="42">
         <v>11</v>
       </c>
       <c r="C116" s="24" t="s">
@@ -39735,7 +39735,7 @@
       <c r="IS116" s="18"/>
     </row>
     <row r="117" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B117" s="41"/>
+      <c r="B117" s="42"/>
       <c r="C117" s="24" t="s">
         <v>37</v>
       </c>
@@ -40257,7 +40257,7 @@
       <c r="IS117" s="26"/>
     </row>
     <row r="118" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B118" s="41">
+      <c r="B118" s="42">
         <v>12</v>
       </c>
       <c r="C118" s="24" t="s">
@@ -40865,7 +40865,7 @@
       <c r="IS118" s="18"/>
     </row>
     <row r="119" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B119" s="41"/>
+      <c r="B119" s="42"/>
       <c r="C119" s="24" t="s">
         <v>37</v>
       </c>
@@ -41471,7 +41471,7 @@
       <c r="IS119" s="26"/>
     </row>
     <row r="120" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B120" s="41">
+      <c r="B120" s="42">
         <v>13</v>
       </c>
       <c r="C120" s="24" t="s">
@@ -42131,7 +42131,7 @@
       <c r="IS120" s="18"/>
     </row>
     <row r="121" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B121" s="41"/>
+      <c r="B121" s="42"/>
       <c r="C121" s="24" t="s">
         <v>37</v>
       </c>
@@ -42789,7 +42789,7 @@
       <c r="IS121" s="26"/>
     </row>
     <row r="122" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B122" s="41">
+      <c r="B122" s="42">
         <v>14</v>
       </c>
       <c r="C122" s="24" t="s">
@@ -43449,7 +43449,7 @@
       <c r="IS122" s="18"/>
     </row>
     <row r="123" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B123" s="41"/>
+      <c r="B123" s="42"/>
       <c r="C123" s="24" t="s">
         <v>37</v>
       </c>
@@ -44107,7 +44107,7 @@
       <c r="IS123" s="26"/>
     </row>
     <row r="124" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B124" s="41">
+      <c r="B124" s="42">
         <v>15</v>
       </c>
       <c r="C124" s="24" t="s">
@@ -44365,7 +44365,7 @@
       <c r="IS124" s="18"/>
     </row>
     <row r="125" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B125" s="41"/>
+      <c r="B125" s="42"/>
       <c r="C125" s="24" t="s">
         <v>37</v>
       </c>
@@ -44621,7 +44621,7 @@
       <c r="IS125" s="26"/>
     </row>
     <row r="126" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B126" s="41">
+      <c r="B126" s="42">
         <v>16</v>
       </c>
       <c r="C126" s="24" t="s">
@@ -44879,7 +44879,7 @@
       <c r="IS126" s="18"/>
     </row>
     <row r="127" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B127" s="41"/>
+      <c r="B127" s="42"/>
       <c r="C127" s="24" t="s">
         <v>37</v>
       </c>
@@ -45135,7 +45135,7 @@
       <c r="IS127" s="26"/>
     </row>
     <row r="128" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B128" s="41">
+      <c r="B128" s="42">
         <v>17</v>
       </c>
       <c r="C128" s="24" t="s">
@@ -45393,7 +45393,7 @@
       <c r="IS128" s="18"/>
     </row>
     <row r="129" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B129" s="41"/>
+      <c r="B129" s="42"/>
       <c r="C129" s="24" t="s">
         <v>37</v>
       </c>
@@ -45649,7 +45649,7 @@
       <c r="IS129" s="26"/>
     </row>
     <row r="130" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B130" s="41">
+      <c r="B130" s="42">
         <v>18</v>
       </c>
       <c r="C130" s="24" t="s">
@@ -45907,7 +45907,7 @@
       <c r="IS130" s="18"/>
     </row>
     <row r="131" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B131" s="41"/>
+      <c r="B131" s="42"/>
       <c r="C131" s="24" t="s">
         <v>37</v>
       </c>
@@ -46163,7 +46163,7 @@
       <c r="IS131" s="26"/>
     </row>
     <row r="132" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B132" s="41">
+      <c r="B132" s="42">
         <v>19</v>
       </c>
       <c r="C132" s="24" t="s">
@@ -46421,7 +46421,7 @@
       <c r="IS132" s="18"/>
     </row>
     <row r="133" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B133" s="41"/>
+      <c r="B133" s="42"/>
       <c r="C133" s="24" t="s">
         <v>37</v>
       </c>
@@ -46677,7 +46677,7 @@
       <c r="IS133" s="26"/>
     </row>
     <row r="134" spans="2:253" x14ac:dyDescent="0.25">
-      <c r="B134" s="41">
+      <c r="B134" s="42">
         <v>20</v>
       </c>
       <c r="C134" s="24" t="s">
@@ -46935,7 +46935,7 @@
       <c r="IS134" s="18"/>
     </row>
     <row r="135" spans="2:253" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="42"/>
+      <c r="B135" s="43"/>
       <c r="C135" s="27" t="s">
         <v>37</v>
       </c>
@@ -47192,14 +47192,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="B120:B121"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="B130:B131"/>
     <mergeCell ref="B118:B119"/>
     <mergeCell ref="B96:B97"/>
     <mergeCell ref="B98:B99"/>
@@ -47212,6 +47204,14 @@
     <mergeCell ref="B112:B113"/>
     <mergeCell ref="B114:B115"/>
     <mergeCell ref="B116:B117"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="B130:B131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>